<commit_message>
-replacing dollar sign with jQuery
</commit_message>
<xml_diff>
--- a/instances/charts/energy/dry11_coal_reserves/coal_reserves_exposure.xlsx
+++ b/instances/charts/energy/dry11_coal_reserves/coal_reserves_exposure.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HT/GoogleDrive/CWR/Projects/2017WebsiteRevamp/github/instances/charts/energy/dry11_coal_reserves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ht/GoogleDrive/CWR/Projects/2017WebsiteRevamp/github/instances/charts/energy/dry11_coal_reserves/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="4220" windowWidth="28560" windowHeight="17380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9840" yWindow="4220" windowWidth="28560" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -17,9 +17,12 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>Province</t>
   </si>
@@ -148,6 +151,21 @@
   </si>
   <si>
     <t>Sum of Coal reserves 2016_2</t>
+  </si>
+  <si>
+    <t>Category2</t>
+  </si>
+  <si>
+    <t>&lt;500 Extreme Water Scarce</t>
+  </si>
+  <si>
+    <t>1000-2000 Water Stress</t>
+  </si>
+  <si>
+    <t>500-1000 Water Scarce</t>
+  </si>
+  <si>
+    <t>&gt;2000 Water Rich</t>
   </si>
 </sst>
 </file>
@@ -207,21 +225,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -270,11 +301,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="CWR" refreshedDate="43285.563449421294" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="31">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43286.862231250001" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="31">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="3">
+  <cacheFields count="4">
     <cacheField name="Province" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -285,40 +316,16 @@
         <s v="Safe 13"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="Category2" numFmtId="0">
+      <sharedItems count="4">
+        <s v="1000-2000 Water Stress"/>
+        <s v="&lt;500 Extreme Water Scarce"/>
+        <s v="&gt;2000 Water Rich"/>
+        <s v="500-1000 Water Scarce"/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="Coal reserves 2016" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.12" maxValue="916.19" count="31">
-        <n v="82.37"/>
-        <n v="2.66"/>
-        <n v="18.03"/>
-        <n v="3.98"/>
-        <n v="27.32"/>
-        <n v="0.23"/>
-        <n v="0.9"/>
-        <n v="110.93"/>
-        <n v="1.19"/>
-        <n v="43.27"/>
-        <n v="62.28"/>
-        <n v="85.58"/>
-        <n v="3.2"/>
-        <n v="6.62"/>
-        <n v="510.27"/>
-        <n v="10.39"/>
-        <n v="3.36"/>
-        <n v="9.7100000000000009"/>
-        <n v="26.73"/>
-        <n v="37.450000000000003"/>
-        <n v="12.39"/>
-        <n v="162.93"/>
-        <n v="75.67"/>
-        <m/>
-        <n v="916.19"/>
-        <n v="53.21"/>
-        <n v="2.97"/>
-        <n v="0.12"/>
-        <n v="162.31"/>
-        <n v="59.58"/>
-        <n v="0.43"/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.12" maxValue="916.19"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -335,164 +342,264 @@
     <s v="Anhui"/>
     <x v="0"/>
     <x v="0"/>
+    <n v="82.37"/>
   </r>
   <r>
     <s v="Beijing"/>
     <x v="1"/>
     <x v="1"/>
+    <n v="2.66"/>
   </r>
   <r>
     <s v="Chongqing"/>
     <x v="0"/>
-    <x v="2"/>
+    <x v="0"/>
+    <n v="18.03"/>
   </r>
   <r>
     <s v="Fujian"/>
     <x v="2"/>
+    <x v="2"/>
+    <n v="3.98"/>
+  </r>
+  <r>
+    <s v="Gansu"/>
+    <x v="1"/>
     <x v="3"/>
-  </r>
-  <r>
-    <s v="Gansu"/>
-    <x v="1"/>
-    <x v="4"/>
+    <n v="27.32"/>
   </r>
   <r>
     <s v="Guangdong"/>
     <x v="0"/>
-    <x v="5"/>
+    <x v="0"/>
+    <n v="0.23"/>
   </r>
   <r>
     <s v="Guangxi"/>
     <x v="2"/>
-    <x v="6"/>
+    <x v="2"/>
+    <n v="0.9"/>
   </r>
   <r>
     <s v="Guizhou"/>
     <x v="2"/>
-    <x v="7"/>
+    <x v="2"/>
+    <n v="110.93"/>
   </r>
   <r>
     <s v="Hainan"/>
     <x v="2"/>
-    <x v="8"/>
+    <x v="2"/>
+    <n v="1.19"/>
   </r>
   <r>
     <s v="Hebei"/>
     <x v="1"/>
-    <x v="9"/>
+    <x v="1"/>
+    <n v="43.27"/>
   </r>
   <r>
     <s v="Heilongjiang"/>
     <x v="2"/>
-    <x v="10"/>
+    <x v="0"/>
+    <n v="62.28"/>
   </r>
   <r>
     <s v="Henan"/>
     <x v="1"/>
-    <x v="11"/>
+    <x v="1"/>
+    <n v="85.58"/>
   </r>
   <r>
     <s v="Hubei"/>
     <x v="0"/>
-    <x v="12"/>
+    <x v="0"/>
+    <n v="3.2"/>
   </r>
   <r>
     <s v="Hunan"/>
     <x v="2"/>
-    <x v="13"/>
+    <x v="2"/>
+    <n v="6.62"/>
   </r>
   <r>
     <s v="Inner Mongolia"/>
     <x v="0"/>
-    <x v="14"/>
+    <x v="0"/>
+    <n v="510.27"/>
   </r>
   <r>
     <s v="Jiangsu"/>
     <x v="1"/>
-    <x v="15"/>
+    <x v="3"/>
+    <n v="10.39"/>
   </r>
   <r>
     <s v="Jiangxi"/>
     <x v="2"/>
-    <x v="16"/>
+    <x v="2"/>
+    <n v="3.36"/>
   </r>
   <r>
     <s v="Jilin"/>
     <x v="0"/>
-    <x v="17"/>
+    <x v="0"/>
+    <n v="9.7100000000000009"/>
   </r>
   <r>
     <s v="Liaoning"/>
     <x v="1"/>
-    <x v="18"/>
+    <x v="3"/>
+    <n v="26.73"/>
   </r>
   <r>
     <s v="Ningxia"/>
     <x v="1"/>
-    <x v="19"/>
+    <x v="1"/>
+    <n v="37.450000000000003"/>
   </r>
   <r>
     <s v="Qinghai"/>
     <x v="2"/>
-    <x v="20"/>
+    <x v="2"/>
+    <n v="12.39"/>
   </r>
   <r>
     <s v="Shaanxi"/>
     <x v="0"/>
-    <x v="21"/>
+    <x v="0"/>
+    <n v="162.93"/>
   </r>
   <r>
     <s v="Shandong"/>
     <x v="1"/>
-    <x v="22"/>
+    <x v="1"/>
+    <n v="75.67"/>
   </r>
   <r>
     <s v="Shanghai"/>
     <x v="1"/>
-    <x v="23"/>
+    <x v="1"/>
+    <m/>
   </r>
   <r>
     <s v="Shanxi"/>
     <x v="1"/>
-    <x v="24"/>
+    <x v="1"/>
+    <n v="916.19"/>
   </r>
   <r>
     <s v="Sichuan"/>
     <x v="2"/>
-    <x v="25"/>
+    <x v="2"/>
+    <n v="53.21"/>
   </r>
   <r>
     <s v="Tianjin"/>
     <x v="1"/>
-    <x v="26"/>
+    <x v="1"/>
+    <n v="2.97"/>
   </r>
   <r>
     <s v="Tibet"/>
     <x v="2"/>
-    <x v="27"/>
+    <x v="2"/>
+    <n v="0.12"/>
   </r>
   <r>
     <s v="Xinjiang"/>
     <x v="2"/>
-    <x v="28"/>
+    <x v="2"/>
+    <n v="162.31"/>
   </r>
   <r>
     <s v="Yunnan"/>
     <x v="2"/>
-    <x v="29"/>
+    <x v="2"/>
+    <n v="59.58"/>
   </r>
   <r>
     <s v="Zhejiang"/>
     <x v="2"/>
-    <x v="30"/>
+    <x v="0"/>
+    <n v="0.43"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A14:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Coal reserves 2016_2" fld="3" baseField="1" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
+  <pivotFields count="4">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -502,42 +609,8 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="32">
-        <item x="27"/>
-        <item x="5"/>
-        <item x="30"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="26"/>
-        <item x="12"/>
-        <item x="16"/>
-        <item x="3"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="15"/>
-        <item x="20"/>
-        <item x="2"/>
-        <item x="18"/>
-        <item x="4"/>
-        <item x="19"/>
-        <item x="9"/>
-        <item x="25"/>
-        <item x="29"/>
-        <item x="10"/>
-        <item x="22"/>
-        <item x="0"/>
-        <item x="11"/>
-        <item x="7"/>
-        <item x="28"/>
-        <item x="21"/>
-        <item x="14"/>
-        <item x="24"/>
-        <item x="23"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
@@ -560,17 +633,17 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Coal reserves 2016_2" fld="2" baseField="1" baseItem="0"/>
+    <dataField name="Sum of Coal reserves 2016_2" fld="3" baseField="1" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -590,11 +663,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0">
-  <autoFilter ref="A1:C32"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Province" dataDxfId="6"/>
-    <tableColumn id="2" name="Category" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0">
+  <autoFilter ref="A1:D32"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Province" dataDxfId="5"/>
+    <tableColumn id="2" name="Category" dataDxfId="4"/>
+    <tableColumn id="4" name="Category2" dataDxfId="3"/>
     <tableColumn id="3" name="Coal reserves 2016"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -864,17 +938,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B7"/>
+  <dimension ref="A3:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
@@ -914,6 +988,54 @@
         <v>38</v>
       </c>
       <c r="B7" s="7">
+        <v>2492.27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1163.7900000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="7">
+        <v>414.59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="7">
+        <v>849.44999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="7">
+        <v>64.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="7">
         <v>2492.27</v>
       </c>
     </row>
@@ -927,431 +1049,496 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="36.5" customWidth="1"/>
+    <col min="4" max="4" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
         <v>82.37</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
         <v>2.66</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
         <v>18.03</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5">
         <v>3.98</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6">
         <v>27.32</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
         <v>0.23</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
         <v>0.9</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9">
         <v>110.93</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
         <v>1.19</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11">
         <v>43.27</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
         <v>62.28</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13">
         <v>85.58</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
         <v>3.2</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15">
         <v>6.62</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16">
         <v>510.27</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
         <v>10.39</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18">
         <v>3.36</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19">
         <v>9.7100000000000009</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
         <v>26.73</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21">
         <v>37.450000000000003</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22">
         <v>12.39</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23">
         <v>162.93</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
         <v>75.67</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26">
         <v>916.19</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
         <v>53.21</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28">
         <v>2.97</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29">
         <v>0.12</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30">
         <v>162.31</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31">
         <v>59.58</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32">
         <v>0.43</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G33" s="1"/>
-      <c r="H33" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>